<commit_message>
dcos: database input 엑셀파일 수정
</commit_message>
<xml_diff>
--- a/BE/App/database_input.xlsx
+++ b/BE/App/database_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crossrunway/CapstoneProject/2/project2team8/BE/App/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42FEA91-921F-9A4D-8640-BB1260B598D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE2E417-F6E3-E541-98B9-7F274C30CBD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7940" yWindow="500" windowWidth="16740" windowHeight="25100" xr2:uid="{C0E22780-85EA-5A4E-B6EE-41CCB5A1A3EF}"/>
+    <workbookView xWindow="28720" yWindow="5560" windowWidth="17480" windowHeight="25100" xr2:uid="{C0E22780-85EA-5A4E-B6EE-41CCB5A1A3EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -253,9 +253,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -594,7 +597,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -604,338 +607,338 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>126380</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>164779</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>1515323</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>877059</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>164742</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>155319</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>126362</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>35636</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>266961</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>688996</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>1160363</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>164788</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>382199</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>155276</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>126256</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>547583</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>536541</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19">
+      <c r="A19" s="1">
         <v>860332</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20">
+      <c r="A20" s="1">
         <v>401731</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21">
+      <c r="A21" s="1">
         <v>120021</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22">
+      <c r="A22" s="1">
         <v>199252</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23">
+      <c r="A23" s="1">
         <v>1133217</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24">
+      <c r="A24" s="1">
         <v>161383</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Feat: Chatbot - getResponse method
</commit_message>
<xml_diff>
--- a/BE/App/database_input.xlsx
+++ b/BE/App/database_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crossrunway/CapstoneProject/2/project2team8/BE/App/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42FEA91-921F-9A4D-8640-BB1260B598D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE2E417-F6E3-E541-98B9-7F274C30CBD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7940" yWindow="500" windowWidth="16740" windowHeight="25100" xr2:uid="{C0E22780-85EA-5A4E-B6EE-41CCB5A1A3EF}"/>
+    <workbookView xWindow="28720" yWindow="5560" windowWidth="17480" windowHeight="25100" xr2:uid="{C0E22780-85EA-5A4E-B6EE-41CCB5A1A3EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -253,9 +253,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -594,7 +597,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -604,338 +607,338 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>126380</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>164779</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>1515323</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>877059</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>164742</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>155319</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>126362</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>35636</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>266961</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>688996</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>1160363</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>164788</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>382199</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>155276</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>126256</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>547583</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>536541</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19">
+      <c r="A19" s="1">
         <v>860332</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20">
+      <c r="A20" s="1">
         <v>401731</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21">
+      <c r="A21" s="1">
         <v>120021</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22">
+      <c r="A22" s="1">
         <v>199252</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23">
+      <c r="A23" s="1">
         <v>1133217</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24">
+      <c r="A24" s="1">
         <v>161383</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor : 폴더 정리 + view.py 에서 Dart 빼기
</commit_message>
<xml_diff>
--- a/BE/App/database_input.xlsx
+++ b/BE/App/database_input.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crossrunway/CapstoneProject/2/project2team8/BE/App/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\8jong\BE\App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE2E417-F6E3-E541-98B9-7F274C30CBD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28720" yWindow="5560" windowWidth="17480" windowHeight="25100" xr2:uid="{C0E22780-85EA-5A4E-B6EE-41CCB5A1A3EF}"/>
+    <workbookView xWindow="28725" yWindow="5565" windowWidth="17475" windowHeight="25095"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="107">
   <si>
     <t>corp_name</t>
   </si>
@@ -207,14 +206,229 @@
   </si>
   <si>
     <t>is_dart</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JOHNSON &amp; JOHNSON</t>
+  </si>
+  <si>
+    <t>Merck &amp; Co., Inc.</t>
+  </si>
+  <si>
+    <t>Apple Inc.</t>
+  </si>
+  <si>
+    <t>HOME DEPOT, INC.</t>
+  </si>
+  <si>
+    <t>UNITEDHEALTH GROUP INC</t>
+  </si>
+  <si>
+    <t>MICROSOFT CORP</t>
+  </si>
+  <si>
+    <t>AMAZON COM INC</t>
+  </si>
+  <si>
+    <t>NVIDIA CORP</t>
+  </si>
+  <si>
+    <t>BERKSHIRE HATHAWAY INC</t>
+  </si>
+  <si>
+    <t>Salesforce, Inc.</t>
+  </si>
+  <si>
+    <t>Mastercard Inc</t>
+  </si>
+  <si>
+    <t>Tesla, Inc.</t>
+  </si>
+  <si>
+    <t>Meta Platforms, Inc.</t>
+  </si>
+  <si>
+    <t>ORACLE CORP</t>
+  </si>
+  <si>
+    <t>VISA INC.</t>
+  </si>
+  <si>
+    <t>AbbVie Inc.</t>
+  </si>
+  <si>
+    <t>Alphabet Inc.</t>
+  </si>
+  <si>
+    <t>ADVANCED MICRO DEVICES INC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JPMORGAN CHASE &amp; CO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXXON MOBIL CORP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엑슨모빌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ELI LILLY &amp; Co</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엘리 릴리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BANK OF AMERICA CORP /DE/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PROCTER &amp; GAMBLE Co</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프록터 앤 갬블</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P&amp;G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Walmart Inc.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>월마트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J&amp;J</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MSD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>머크</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>애플</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>홈디포</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유나이티드헬스그룹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뱅크오브아메리카</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>존슨앤존슨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마이크로소프트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COSTCO WHOLESALE CORP /NEW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>코스트코</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아마존</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엔비디아</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>버크셔해서웨이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세일즈포스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마스터카드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>테슬라</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메타</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오라클</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>애브비</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>알파벳</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Broadcom Inc.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>브로드컴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JP모건체이스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에이엠디</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>페이스북</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구글</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -227,6 +441,21 @@
       <sz val="8"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -253,11 +482,20 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -593,20 +831,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A36F0152-7C36-3949-A939-54AF72EBCF58}">
-  <dimension ref="A1:D24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -620,7 +859,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>126380</v>
       </c>
@@ -634,7 +873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>164779</v>
       </c>
@@ -648,7 +887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1515323</v>
       </c>
@@ -662,7 +901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>877059</v>
       </c>
@@ -676,7 +915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>164742</v>
       </c>
@@ -690,7 +929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>155319</v>
       </c>
@@ -704,7 +943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>126362</v>
       </c>
@@ -718,7 +957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>35636</v>
       </c>
@@ -732,7 +971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>266961</v>
       </c>
@@ -746,7 +985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>688996</v>
       </c>
@@ -760,7 +999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>1160363</v>
       </c>
@@ -774,7 +1013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>164788</v>
       </c>
@@ -788,7 +1027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>382199</v>
       </c>
@@ -802,7 +1041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>155276</v>
       </c>
@@ -816,7 +1055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>126256</v>
       </c>
@@ -830,7 +1069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>547583</v>
       </c>
@@ -844,7 +1083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>536541</v>
       </c>
@@ -858,7 +1097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>860332</v>
       </c>
@@ -872,7 +1111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>401731</v>
       </c>
@@ -886,7 +1125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>120021</v>
       </c>
@@ -900,7 +1139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>199252</v>
       </c>
@@ -914,7 +1153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>1133217</v>
       </c>
@@ -928,7 +1167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>161383</v>
       </c>
@@ -940,10 +1179,315 @@
       </c>
       <c r="D24" s="1">
         <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D42" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D43" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
docs: database input 자료확정
</commit_message>
<xml_diff>
--- a/BE/App/database_input.xlsx
+++ b/BE/App/database_input.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\8jong\BE\App\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crossrunway/Projects/project2team8/BE/App/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE6BFDF-057C-8D4E-8F24-7446A6A12042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28725" yWindow="5565" windowWidth="17475" windowHeight="25095"/>
+    <workbookView xWindow="-17720" yWindow="14440" windowWidth="17480" windowHeight="25100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="127">
   <si>
     <t>corp_name</t>
   </si>
@@ -300,10 +290,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>P&amp;G</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Walmart Inc.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -312,18 +298,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>J&amp;J</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MSD</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>머크</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>애플</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -412,23 +390,115 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>에이엠디</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>페이스북</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>구글</t>
+    <t>0000019617</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000034088</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000059478</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000070858</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000080424</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000200406</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000310158</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000320193</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000354950</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000731766</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000789019</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000909832</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001018724</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001045810</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000104169</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001067983</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001108524</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001141391</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001318605</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001326801</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001341439</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001403161</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001551152</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001652044</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001730168</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000002488</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -489,13 +559,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -831,21 +901,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="143" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -859,7 +929,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>126380</v>
       </c>
@@ -873,7 +943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>164779</v>
       </c>
@@ -887,7 +957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>1515323</v>
       </c>
@@ -901,7 +971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>877059</v>
       </c>
@@ -915,7 +985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>164742</v>
       </c>
@@ -929,7 +999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>155319</v>
       </c>
@@ -943,7 +1013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>126362</v>
       </c>
@@ -957,7 +1027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>35636</v>
       </c>
@@ -971,7 +1041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>266961</v>
       </c>
@@ -985,7 +1055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>688996</v>
       </c>
@@ -999,7 +1069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>1160363</v>
       </c>
@@ -1013,7 +1083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="A13" s="1">
         <v>164788</v>
       </c>
@@ -1027,7 +1097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="A14" s="1">
         <v>382199</v>
       </c>
@@ -1041,7 +1111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>155276</v>
       </c>
@@ -1055,7 +1125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="A16" s="1">
         <v>126256</v>
       </c>
@@ -1069,7 +1139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>547583</v>
       </c>
@@ -1083,7 +1153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>536541</v>
       </c>
@@ -1097,7 +1167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>860332</v>
       </c>
@@ -1111,7 +1181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>401731</v>
       </c>
@@ -1125,7 +1195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>120021</v>
       </c>
@@ -1139,7 +1209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>199252</v>
       </c>
@@ -1153,7 +1223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4">
       <c r="A23" s="1">
         <v>1133217</v>
       </c>
@@ -1167,7 +1237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4">
       <c r="A24" s="1">
         <v>161383</v>
       </c>
@@ -1181,305 +1251,365 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:4">
+      <c r="A25" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="D25" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>103</v>
+    <row r="26" spans="1:4">
+      <c r="A26" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="C26" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="D26" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>70</v>
+    <row r="27" spans="1:4">
+      <c r="A27" s="4" t="s">
+        <v>102</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="C27" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="D27" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>72</v>
+    <row r="28" spans="1:4">
+      <c r="A28" s="4" t="s">
+        <v>103</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="C28" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="D28" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>85</v>
+    <row r="29" spans="1:4">
+      <c r="A29" s="4" t="s">
+        <v>104</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="C29" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="D29" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>75</v>
+    <row r="30" spans="1:4">
+      <c r="A30" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>77</v>
       </c>
       <c r="D31" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>86</v>
+    <row r="32" spans="1:4">
+      <c r="A32" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D32" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>80</v>
+    <row r="33" spans="1:4">
+      <c r="A33" s="4" t="s">
+        <v>107</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D33" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>82</v>
+    <row r="34" spans="1:4">
+      <c r="A34" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="C34" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="D34" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>83</v>
+    <row r="35" spans="1:4">
+      <c r="A35" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="C35" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="D35" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>84</v>
+    <row r="36" spans="1:4">
+      <c r="A36" s="4" t="s">
+        <v>110</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="C36" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="D36" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>87</v>
+    <row r="37" spans="1:4">
+      <c r="A37" s="4" t="s">
+        <v>111</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="C37" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="D37" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>89</v>
+    <row r="38" spans="1:4">
+      <c r="A38" s="4" t="s">
+        <v>112</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="D38" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
-        <v>90</v>
+    <row r="39" spans="1:4">
+      <c r="A39" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="C39" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="D39" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
-        <v>91</v>
+    <row r="40" spans="1:4">
+      <c r="A40" s="4" t="s">
+        <v>114</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="C40" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="D40" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
-        <v>92</v>
+    <row r="41" spans="1:4">
+      <c r="A41" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="C41" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="D41" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
-        <v>93</v>
+    <row r="42" spans="1:4">
+      <c r="A42" s="4" t="s">
+        <v>117</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="C42" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="D42" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
-        <v>94</v>
+    <row r="43" spans="1:4">
+      <c r="A43" s="4" t="s">
+        <v>118</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="C43" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="D43" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>95</v>
+    <row r="44" spans="1:4">
+      <c r="A44" s="4" t="s">
+        <v>119</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="C44" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="D44" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
-        <v>96</v>
+    <row r="45" spans="1:4">
+      <c r="A45" s="4" t="s">
+        <v>120</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="D45" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
-        <v>97</v>
+    <row r="46" spans="1:4">
+      <c r="A46" s="4" t="s">
+        <v>121</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="C46" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="D46" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
-        <v>98</v>
+    <row r="47" spans="1:4">
+      <c r="A47" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="C47" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="D47" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>99</v>
+    <row r="48" spans="1:4">
+      <c r="A48" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="C48" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="D48" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
-        <v>100</v>
+    <row r="49" spans="1:4">
+      <c r="A49" s="4" t="s">
+        <v>124</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D49" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
-        <v>102</v>
+    <row r="50" spans="1:4">
+      <c r="A50" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="D50" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
docs: database 자료 변경
</commit_message>
<xml_diff>
--- a/BE/App/database_input.xlsx
+++ b/BE/App/database_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crossrunway/Projects/project2team8/BE/App/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE6BFDF-057C-8D4E-8F24-7446A6A12042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4948BBA7-155E-C844-99F5-C8B9B3418FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17720" yWindow="14440" windowWidth="17480" windowHeight="25100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-17720" yWindow="14420" windowWidth="17480" windowHeight="25100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -205,292 +205,293 @@
     <t>Merck &amp; Co., Inc.</t>
   </si>
   <si>
+    <t>HOME DEPOT, INC.</t>
+  </si>
+  <si>
+    <t>UNITEDHEALTH GROUP INC</t>
+  </si>
+  <si>
+    <t>MICROSOFT CORP</t>
+  </si>
+  <si>
+    <t>AMAZON COM INC</t>
+  </si>
+  <si>
+    <t>NVIDIA CORP</t>
+  </si>
+  <si>
+    <t>BERKSHIRE HATHAWAY INC</t>
+  </si>
+  <si>
+    <t>Salesforce, Inc.</t>
+  </si>
+  <si>
+    <t>Mastercard Inc</t>
+  </si>
+  <si>
+    <t>Tesla, Inc.</t>
+  </si>
+  <si>
+    <t>Meta Platforms, Inc.</t>
+  </si>
+  <si>
+    <t>ORACLE CORP</t>
+  </si>
+  <si>
+    <t>VISA INC.</t>
+  </si>
+  <si>
+    <t>AbbVie Inc.</t>
+  </si>
+  <si>
+    <t>Alphabet Inc.</t>
+  </si>
+  <si>
+    <t>ADVANCED MICRO DEVICES INC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JPMORGAN CHASE &amp; CO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXXON MOBIL CORP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엑슨모빌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ELI LILLY &amp; Co</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엘리 릴리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BANK OF AMERICA CORP /DE/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PROCTER &amp; GAMBLE Co</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프록터 앤 갬블</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Walmart Inc.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>월마트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MSD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>애플</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>홈디포</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유나이티드헬스그룹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뱅크오브아메리카</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>존슨앤존슨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마이크로소프트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COSTCO WHOLESALE CORP /NEW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>코스트코</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아마존</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엔비디아</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>버크셔해서웨이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세일즈포스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마스터카드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>테슬라</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메타</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오라클</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>애브비</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>알파벳</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Broadcom Inc.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>브로드컴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JP모건체이스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000019617</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000034088</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000059478</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000070858</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000080424</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000200406</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000310158</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000320193</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000354950</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000731766</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000789019</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000909832</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001018724</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001045810</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000104169</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001067983</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001108524</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001141391</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001318605</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001326801</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001341439</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001403161</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001551152</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001652044</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001730168</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000002488</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Apple Inc.</t>
-  </si>
-  <si>
-    <t>HOME DEPOT, INC.</t>
-  </si>
-  <si>
-    <t>UNITEDHEALTH GROUP INC</t>
-  </si>
-  <si>
-    <t>MICROSOFT CORP</t>
-  </si>
-  <si>
-    <t>AMAZON COM INC</t>
-  </si>
-  <si>
-    <t>NVIDIA CORP</t>
-  </si>
-  <si>
-    <t>BERKSHIRE HATHAWAY INC</t>
-  </si>
-  <si>
-    <t>Salesforce, Inc.</t>
-  </si>
-  <si>
-    <t>Mastercard Inc</t>
-  </si>
-  <si>
-    <t>Tesla, Inc.</t>
-  </si>
-  <si>
-    <t>Meta Platforms, Inc.</t>
-  </si>
-  <si>
-    <t>ORACLE CORP</t>
-  </si>
-  <si>
-    <t>VISA INC.</t>
-  </si>
-  <si>
-    <t>AbbVie Inc.</t>
-  </si>
-  <si>
-    <t>Alphabet Inc.</t>
-  </si>
-  <si>
-    <t>ADVANCED MICRO DEVICES INC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AMD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JPMORGAN CHASE &amp; CO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EXXON MOBIL CORP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>엑슨모빌</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ELI LILLY &amp; Co</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>엘리 릴리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BANK OF AMERICA CORP /DE/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PROCTER &amp; GAMBLE Co</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>프록터 앤 갬블</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Walmart Inc.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>월마트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MSD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>애플</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>홈디포</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>유나이티드헬스그룹</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>뱅크오브아메리카</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>존슨앤존슨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>마이크로소프트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>COSTCO WHOLESALE CORP /NEW</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>코스트코</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아마존</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>엔비디아</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>버크셔해서웨이</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>세일즈포스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>마스터카드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>테슬라</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>메타</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오라클</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>비자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>애브비</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>알파벳</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Broadcom Inc.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>브로드컴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JP모건체이스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0000019617</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0000034088</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0000059478</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0000070858</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0000080424</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0000200406</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0000310158</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0000320193</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0000354950</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0000731766</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0000789019</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0000909832</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0001018724</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0001045810</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0000104169</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0001067983</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0001108524</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0001141391</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0001318605</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0001326801</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0001341439</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0001403161</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0001551152</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0001652044</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0001730168</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0000002488</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -904,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="143" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="143" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="18"/>
@@ -1253,13 +1254,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="D25" s="1">
         <v>0</v>
@@ -1267,13 +1268,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D26" s="1">
         <v>0</v>
@@ -1281,13 +1282,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="D27" s="1">
         <v>0</v>
@@ -1295,13 +1296,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="D28" s="1">
         <v>0</v>
@@ -1309,13 +1310,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D29" s="1">
         <v>0</v>
@@ -1323,13 +1324,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="D30" s="1">
         <v>0</v>
@@ -1337,13 +1338,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="D31" s="1">
         <v>0</v>
@@ -1351,13 +1352,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D32" s="1">
         <v>0</v>
@@ -1365,13 +1366,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D33" s="1">
         <v>0</v>
@@ -1379,13 +1380,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D34" s="1">
         <v>0</v>
@@ -1393,13 +1394,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D35" s="1">
         <v>0</v>
@@ -1407,13 +1408,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D36" s="1">
         <v>0</v>
@@ -1421,13 +1422,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D37" s="1">
         <v>0</v>
@@ -1435,13 +1436,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="D38" s="1">
         <v>0</v>
@@ -1449,13 +1450,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D39" s="1">
         <v>0</v>
@@ -1463,13 +1464,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D40" s="1">
         <v>0</v>
@@ -1477,13 +1478,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D41" s="1">
         <v>0</v>
@@ -1491,13 +1492,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D42" s="1">
         <v>0</v>
@@ -1505,13 +1506,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D43" s="1">
         <v>0</v>
@@ -1519,13 +1520,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D44" s="1">
         <v>0</v>
@@ -1533,13 +1534,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D45" s="1">
         <v>0</v>
@@ -1547,13 +1548,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D46" s="1">
         <v>0</v>
@@ -1561,13 +1562,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D47" s="1">
         <v>0</v>
@@ -1575,13 +1576,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D48" s="1">
         <v>0</v>
@@ -1589,13 +1590,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D49" s="1">
         <v>0</v>
@@ -1603,13 +1604,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="D50" s="1">
         <v>0</v>

</xml_diff>